<commit_message>
Lista maestro de requerimientos finalizada
</commit_message>
<xml_diff>
--- a/Recursos/Nomenclaturas.xlsx
+++ b/Recursos/Nomenclaturas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Desarrollo 2\Documentacion\Entregable 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Desarrollo 2\Documentacion\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="6465" windowHeight="3420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6465" windowHeight="3420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1462,7 +1462,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>